<commit_message>
adding absorbance calculations to processNCR.R.
</commit_message>
<xml_diff>
--- a/exampleData.xlsx
+++ b/exampleData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-23740" yWindow="-15840" windowWidth="25600" windowHeight="15540"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="exampleData" sheetId="1" r:id="rId1"/>
@@ -1019,7 +1019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="92" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="92" workbookViewId="0">
       <selection activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>

</xml_diff>